<commit_message>
test xing neng on 6.30
</commit_message>
<xml_diff>
--- a/src/dependence/test.xlsx
+++ b/src/dependence/test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24321" uniqueCount="7217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23979" uniqueCount="7204">
   <si>
     <t>D:/third_party/openalpr-2.3.0/Task3_车牌识别/功能评测图像库/车牌种类变化子库/testImg/GL61690.jpg</t>
   </si>
@@ -21626,45 +21626,6 @@
   </si>
   <si>
     <t>警C2128学</t>
-  </si>
-  <si>
-    <t>京A08N14</t>
-  </si>
-  <si>
-    <t>京A30258</t>
-  </si>
-  <si>
-    <t>京F49R29</t>
-  </si>
-  <si>
-    <t>京G6E451</t>
-  </si>
-  <si>
-    <t>京J19630</t>
-  </si>
-  <si>
-    <t>京J4U97B</t>
-  </si>
-  <si>
-    <t>京J62771</t>
-  </si>
-  <si>
-    <t>京K316D2</t>
-  </si>
-  <si>
-    <t>京K36612</t>
-  </si>
-  <si>
-    <t>京K38095</t>
-  </si>
-  <si>
-    <t>京M08M81</t>
-  </si>
-  <si>
-    <t>京M71696</t>
-  </si>
-  <si>
-    <t>京N98H81</t>
   </si>
 </sst>
 </file>
@@ -21996,145 +21957,145 @@
   <sheetData>
     <row r="2">
       <c r="A2" t="s">
-        <v>7204</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>1853</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7205</v>
+        <v>7037</v>
       </c>
       <c r="B3" t="s">
-        <v>2217</v>
+        <v>6155</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6091</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>199</v>
+        <v>1855</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>7039</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>6155</v>
       </c>
       <c r="C5" t="s">
-        <v>200</v>
+        <v>1856</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>6092</v>
+        <v>7187</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C6" t="s">
-        <v>201</v>
+        <v>1857</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6093</v>
+        <v>7188</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>6094</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
+        <v>1859</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7206</v>
+        <v>7189</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C9" t="s">
-        <v>204</v>
+        <v>1860</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>6095</v>
+        <v>7190</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>1861</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6096</v>
+        <v>7191</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C11" t="s">
-        <v>206</v>
+        <v>1862</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>6097</v>
+        <v>7192</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C12" t="s">
-        <v>207</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>6098</v>
+        <v>7193</v>
       </c>
       <c r="B13" t="s">
-        <v>2217</v>
+        <v>6155</v>
       </c>
       <c r="C13" t="s">
-        <v>208</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>7207</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>209</v>
+        <v>1865</v>
       </c>
     </row>
     <row r="15">
@@ -22145,403 +22106,277 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>210</v>
+        <v>1866</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>6100</v>
+        <v>7194</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C16" t="s">
-        <v>211</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>6101</v>
+        <v>7195</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C17" t="s">
-        <v>212</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>6102</v>
+        <v>7045</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>1869</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>6103</v>
+        <v>7196</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C19" t="s">
-        <v>214</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>6104</v>
+        <v>7197</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C20" t="s">
-        <v>215</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>6105</v>
+        <v>7198</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C21" t="s">
-        <v>216</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>6106</v>
+        <v>7199</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C22" t="s">
-        <v>217</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>6107</v>
+        <v>7200</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C23" t="s">
-        <v>218</v>
+        <v>1874</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>7208</v>
+        <v>7049</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C24" t="s">
-        <v>219</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>6109</v>
+        <v>7050</v>
       </c>
       <c r="B25" t="s">
-        <v>2217</v>
+        <v>6155</v>
       </c>
       <c r="C25" t="s">
-        <v>220</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>7201</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>6155</v>
       </c>
       <c r="C26" t="s">
-        <v>221</v>
+        <v>1877</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>6110</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>222</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>7209</v>
+        <v>7202</v>
       </c>
       <c r="B28" t="s">
-        <v>28</v>
+        <v>6155</v>
       </c>
       <c r="C28" t="s">
-        <v>223</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>7210</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>224</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>6112</v>
+        <v>7203</v>
       </c>
       <c r="B30" t="s">
-        <v>2217</v>
+        <v>6155</v>
       </c>
       <c r="C30" t="s">
-        <v>225</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="s">
-        <v>6113</v>
-      </c>
-      <c r="B31" t="s">
-        <v>28</v>
-      </c>
       <c r="C31" t="s">
-        <v>226</v>
+        <v>1882</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="s">
-        <v>6114</v>
-      </c>
-      <c r="B32" t="s">
-        <v>28</v>
-      </c>
       <c r="C32" t="s">
-        <v>227</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s">
-        <v>6115</v>
-      </c>
-      <c r="B33" t="s">
-        <v>28</v>
-      </c>
       <c r="C33" t="s">
-        <v>228</v>
+        <v>1884</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="s">
-        <v>6116</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2217</v>
-      </c>
       <c r="C34" t="s">
-        <v>229</v>
+        <v>1885</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="s">
-        <v>7211</v>
-      </c>
-      <c r="B35" t="s">
-        <v>28</v>
-      </c>
       <c r="C35" t="s">
-        <v>230</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="s">
-        <v>7212</v>
-      </c>
-      <c r="B36" t="s">
-        <v>28</v>
-      </c>
       <c r="C36" t="s">
-        <v>231</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="s">
-        <v>7213</v>
-      </c>
-      <c r="B37" t="s">
-        <v>28</v>
-      </c>
       <c r="C37" t="s">
-        <v>232</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="s">
-        <v>6120</v>
-      </c>
-      <c r="B38" t="s">
-        <v>28</v>
-      </c>
       <c r="C38" t="s">
-        <v>233</v>
+        <v>1889</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="s">
-        <v>6121</v>
-      </c>
-      <c r="B39" t="s">
-        <v>28</v>
-      </c>
       <c r="C39" t="s">
-        <v>234</v>
+        <v>1890</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="s">
-        <v>6122</v>
-      </c>
-      <c r="B40" t="s">
-        <v>28</v>
-      </c>
       <c r="C40" t="s">
-        <v>235</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="s">
-        <v>6123</v>
-      </c>
-      <c r="B41" t="s">
-        <v>28</v>
-      </c>
       <c r="C41" t="s">
-        <v>236</v>
+        <v>1892</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="s">
-        <v>7214</v>
-      </c>
-      <c r="B42" t="s">
-        <v>28</v>
-      </c>
       <c r="C42" t="s">
-        <v>237</v>
+        <v>1893</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="s">
-        <v>6124</v>
-      </c>
-      <c r="B43" t="s">
-        <v>28</v>
-      </c>
       <c r="C43" t="s">
-        <v>238</v>
+        <v>1894</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" t="s">
-        <v>26</v>
-      </c>
       <c r="C44" t="s">
-        <v>239</v>
+        <v>1895</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="s">
-        <v>7215</v>
-      </c>
-      <c r="B45" t="s">
-        <v>28</v>
-      </c>
       <c r="C45" t="s">
-        <v>240</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="s">
-        <v>6126</v>
-      </c>
-      <c r="B46" t="s">
-        <v>28</v>
-      </c>
       <c r="C46" t="s">
-        <v>241</v>
+        <v>1897</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="s">
-        <v>6127</v>
-      </c>
-      <c r="B47" t="s">
-        <v>28</v>
-      </c>
       <c r="C47" t="s">
-        <v>242</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="s">
-        <v>6128</v>
-      </c>
-      <c r="B48" t="s">
-        <v>28</v>
-      </c>
       <c r="C48" t="s">
-        <v>243</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="s">
-        <v>6129</v>
-      </c>
-      <c r="B49" t="s">
-        <v>28</v>
-      </c>
       <c r="C49" t="s">
-        <v>244</v>
+        <v>1900</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s">
-        <v>26</v>
-      </c>
-      <c r="B50" t="s">
-        <v>26</v>
-      </c>
       <c r="C50" t="s">
-        <v>245</v>
+        <v>1901</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="s">
-        <v>7216</v>
-      </c>
-      <c r="B51" t="s">
-        <v>28</v>
-      </c>
       <c r="C51" t="s">
-        <v>246</v>
+        <v>1902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>